<commit_message>
Fixing commit and data entry
</commit_message>
<xml_diff>
--- a/FCAT_Ants.xlsx
+++ b/FCAT_Ants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boloq\Box\Dissertation\FCAT\FCAT_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0F8B74-86FC-410D-8928-0D79B11C661E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2CAC83-E281-4114-9DC1-B95AF12BB023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{AEE42267-113E-7441-A597-CCFC7364CD25}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1917" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="91">
   <si>
     <t>Site</t>
   </si>
@@ -308,7 +308,7 @@
     <t xml:space="preserve">Genera </t>
   </si>
   <si>
-    <t>Wasmania</t>
+    <t>Wasmannia</t>
   </si>
 </sst>
 </file>
@@ -681,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96040816-BCB9-584A-AA65-92DB85A62C15}">
-  <dimension ref="A1:N233"/>
+  <dimension ref="A1:N234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="K233" sqref="K233"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107:XFD107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="16.100000000000001" x14ac:dyDescent="0.35"/>
@@ -3799,7 +3799,7 @@
         <v>5</v>
       </c>
       <c r="C107" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H107" t="s">
         <v>38</v>
@@ -3811,10 +3811,13 @@
         <v>7</v>
       </c>
       <c r="K107" t="s">
-        <v>9</v>
-      </c>
-      <c r="N107" t="s">
-        <v>18</v>
+        <v>90</v>
+      </c>
+      <c r="L107" t="s">
+        <v>24</v>
+      </c>
+      <c r="M107">
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.35">
@@ -3822,7 +3825,7 @@
         <v>8</v>
       </c>
       <c r="B108">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C108" t="s">
         <v>15</v>
@@ -3837,10 +3840,10 @@
         <v>7</v>
       </c>
       <c r="K108" t="s">
-        <v>58</v>
-      </c>
-      <c r="M108">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="N108" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.35">
@@ -3848,7 +3851,7 @@
         <v>8</v>
       </c>
       <c r="B109">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C109" t="s">
         <v>15</v>
@@ -3871,19 +3874,13 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>19</v>
-      </c>
-      <c r="B110" t="s">
-        <v>52</v>
+        <v>8</v>
+      </c>
+      <c r="B110">
+        <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>28</v>
-      </c>
-      <c r="F110" t="s">
-        <v>87</v>
-      </c>
-      <c r="G110" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="H110" t="s">
         <v>38</v>
@@ -3895,24 +3892,27 @@
         <v>7</v>
       </c>
       <c r="K110" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="M110">
         <v>1</v>
       </c>
-      <c r="N110" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>8</v>
-      </c>
-      <c r="B111">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="B111" t="s">
+        <v>52</v>
       </c>
       <c r="C111" t="s">
-        <v>43</v>
+        <v>28</v>
+      </c>
+      <c r="F111" t="s">
+        <v>87</v>
+      </c>
+      <c r="G111" t="s">
+        <v>87</v>
       </c>
       <c r="H111" t="s">
         <v>38</v>
@@ -3929,13 +3929,16 @@
       <c r="M111">
         <v>1</v>
       </c>
+      <c r="N111" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>8</v>
       </c>
       <c r="B112">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C112" t="s">
         <v>43</v>
@@ -3958,37 +3961,31 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>19</v>
-      </c>
-      <c r="B113" t="s">
-        <v>42</v>
+        <v>8</v>
+      </c>
+      <c r="B113">
+        <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>9</v>
-      </c>
-      <c r="F113" t="s">
-        <v>87</v>
-      </c>
-      <c r="G113" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="H113" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I113" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="J113" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K113" t="s">
-        <v>48</v>
-      </c>
-      <c r="M113" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="114" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+      <c r="M113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>19</v>
       </c>
@@ -3998,8 +3995,6 @@
       <c r="C114" t="s">
         <v>9</v>
       </c>
-      <c r="D114"/>
-      <c r="E114"/>
       <c r="F114" t="s">
         <v>87</v>
       </c>
@@ -4018,22 +4013,22 @@
       <c r="K114" t="s">
         <v>48</v>
       </c>
-      <c r="L114"/>
       <c r="M114" t="s">
         <v>9</v>
       </c>
-      <c r="N114"/>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="115" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>19</v>
       </c>
       <c r="B115" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C115" t="s">
-        <v>28</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D115"/>
+      <c r="E115"/>
       <c r="F115" t="s">
         <v>87</v>
       </c>
@@ -4044,7 +4039,7 @@
         <v>88</v>
       </c>
       <c r="I115" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="J115" t="s">
         <v>73</v>
@@ -4052,9 +4047,11 @@
       <c r="K115" t="s">
         <v>48</v>
       </c>
+      <c r="L115"/>
       <c r="M115" t="s">
         <v>9</v>
       </c>
+      <c r="N115"/>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
@@ -4157,10 +4154,10 @@
         <v>19</v>
       </c>
       <c r="B119" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="C119" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F119" t="s">
         <v>87</v>
@@ -4221,10 +4218,10 @@
         <v>19</v>
       </c>
       <c r="B121" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C121" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F121" t="s">
         <v>87</v>
@@ -4233,45 +4230,51 @@
         <v>87</v>
       </c>
       <c r="H121" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I121" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J121" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K121" t="s">
         <v>48</v>
       </c>
-      <c r="M121">
-        <v>1</v>
+      <c r="M121" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>8</v>
-      </c>
-      <c r="B122">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="B122" t="s">
+        <v>40</v>
       </c>
       <c r="C122" t="s">
         <v>28</v>
       </c>
+      <c r="F122" t="s">
+        <v>87</v>
+      </c>
+      <c r="G122" t="s">
+        <v>87</v>
+      </c>
       <c r="H122" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I122" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J122" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K122" t="s">
         <v>48</v>
       </c>
-      <c r="M122" t="s">
-        <v>9</v>
+      <c r="M122">
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.35">
@@ -4282,22 +4285,22 @@
         <v>2</v>
       </c>
       <c r="C123" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H123" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I123" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J123" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K123" t="s">
         <v>48</v>
       </c>
-      <c r="M123">
-        <v>2</v>
+      <c r="M123" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.35">
@@ -4308,22 +4311,22 @@
         <v>2</v>
       </c>
       <c r="C124" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="H124" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I124" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="J124" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K124" t="s">
         <v>48</v>
       </c>
-      <c r="M124" t="s">
-        <v>9</v>
+      <c r="M124">
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.35">
@@ -4331,25 +4334,25 @@
         <v>8</v>
       </c>
       <c r="B125">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C125" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="H125" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I125" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="J125" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K125" t="s">
         <v>48</v>
       </c>
-      <c r="M125">
-        <v>2</v>
+      <c r="M125" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.35">
@@ -4363,19 +4366,19 @@
         <v>37</v>
       </c>
       <c r="H126" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I126" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J126" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K126" t="s">
         <v>48</v>
       </c>
-      <c r="M126" t="s">
-        <v>9</v>
+      <c r="M126">
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.35">
@@ -4386,7 +4389,7 @@
         <v>3</v>
       </c>
       <c r="C127" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H127" t="s">
         <v>88</v>
@@ -4438,16 +4441,16 @@
         <v>3</v>
       </c>
       <c r="C129" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="H129" t="s">
         <v>88</v>
       </c>
       <c r="I129" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="J129" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K129" t="s">
         <v>48</v>
@@ -4461,19 +4464,19 @@
         <v>8</v>
       </c>
       <c r="B130">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C130" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="H130" t="s">
         <v>88</v>
       </c>
       <c r="I130" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="J130" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K130" t="s">
         <v>48</v>
@@ -4490,13 +4493,13 @@
         <v>4</v>
       </c>
       <c r="C131" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="H131" t="s">
         <v>88</v>
       </c>
       <c r="I131" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="J131" t="s">
         <v>73</v>
@@ -4513,25 +4516,25 @@
         <v>8</v>
       </c>
       <c r="B132">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="H132" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I132" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="J132" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K132" t="s">
         <v>48</v>
       </c>
-      <c r="M132">
-        <v>5</v>
+      <c r="M132" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.35">
@@ -4545,19 +4548,19 @@
         <v>28</v>
       </c>
       <c r="H133" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I133" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J133" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K133" t="s">
         <v>48</v>
       </c>
-      <c r="M133" t="s">
-        <v>9</v>
+      <c r="M133">
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.35">
@@ -4568,7 +4571,7 @@
         <v>5</v>
       </c>
       <c r="C134" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="H134" t="s">
         <v>88</v>
@@ -4594,54 +4597,48 @@
         <v>5</v>
       </c>
       <c r="C135" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="H135" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I135" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J135" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K135" t="s">
         <v>48</v>
       </c>
-      <c r="M135">
-        <v>1</v>
+      <c r="M135" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>19</v>
-      </c>
-      <c r="B136" t="s">
-        <v>20</v>
+        <v>8</v>
+      </c>
+      <c r="B136">
+        <v>5</v>
       </c>
       <c r="C136" t="s">
-        <v>9</v>
-      </c>
-      <c r="F136" t="s">
-        <v>87</v>
-      </c>
-      <c r="G136" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="H136" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I136" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="J136" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K136" t="s">
-        <v>54</v>
-      </c>
-      <c r="M136" t="s">
-        <v>9</v>
+        <v>48</v>
+      </c>
+      <c r="M136">
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.35">
@@ -4649,7 +4646,7 @@
         <v>19</v>
       </c>
       <c r="B137" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="C137" t="s">
         <v>9</v>
@@ -4667,7 +4664,7 @@
         <v>70</v>
       </c>
       <c r="J137" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K137" t="s">
         <v>54</v>
@@ -4681,7 +4678,7 @@
         <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C138" t="s">
         <v>9</v>
@@ -4699,7 +4696,7 @@
         <v>70</v>
       </c>
       <c r="J138" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K138" t="s">
         <v>54</v>
@@ -4713,10 +4710,10 @@
         <v>19</v>
       </c>
       <c r="B139" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="C139" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F139" t="s">
         <v>87</v>
@@ -4725,30 +4722,36 @@
         <v>87</v>
       </c>
       <c r="H139" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I139" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="J139" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K139" t="s">
         <v>54</v>
       </c>
-      <c r="M139">
-        <v>1</v>
+      <c r="M139" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>8</v>
-      </c>
-      <c r="B140">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="B140" t="s">
+        <v>52</v>
       </c>
       <c r="C140" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="F140" t="s">
+        <v>87</v>
+      </c>
+      <c r="G140" t="s">
+        <v>87</v>
       </c>
       <c r="H140" t="s">
         <v>38</v>
@@ -4774,22 +4777,22 @@
         <v>2</v>
       </c>
       <c r="C141" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H141" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I141" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J141" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K141" t="s">
         <v>54</v>
       </c>
-      <c r="M141" t="s">
-        <v>9</v>
+      <c r="M141">
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.35">
@@ -4800,13 +4803,13 @@
         <v>2</v>
       </c>
       <c r="C142" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H142" t="s">
         <v>88</v>
       </c>
       <c r="I142" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="J142" t="s">
         <v>73</v>
@@ -4823,16 +4826,16 @@
         <v>8</v>
       </c>
       <c r="B143">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C143" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="H143" t="s">
         <v>88</v>
       </c>
       <c r="I143" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="J143" t="s">
         <v>73</v>
@@ -4852,13 +4855,13 @@
         <v>4</v>
       </c>
       <c r="C144" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H144" t="s">
         <v>88</v>
       </c>
       <c r="I144" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="J144" t="s">
         <v>73</v>
@@ -4872,34 +4875,28 @@
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>19</v>
-      </c>
-      <c r="B145" t="s">
-        <v>42</v>
+        <v>8</v>
+      </c>
+      <c r="B145">
+        <v>4</v>
       </c>
       <c r="C145" t="s">
-        <v>15</v>
-      </c>
-      <c r="F145" t="s">
-        <v>87</v>
-      </c>
-      <c r="G145" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="H145" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I145" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="J145" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K145" t="s">
-        <v>46</v>
-      </c>
-      <c r="M145">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="M145" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.35">
@@ -4907,10 +4904,10 @@
         <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C146" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="F146" t="s">
         <v>87</v>
@@ -4931,7 +4928,7 @@
         <v>46</v>
       </c>
       <c r="M146">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.35">
@@ -4942,7 +4939,7 @@
         <v>20</v>
       </c>
       <c r="C147" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F147" t="s">
         <v>87</v>
@@ -4963,7 +4960,7 @@
         <v>46</v>
       </c>
       <c r="M147">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.35">
@@ -4974,7 +4971,7 @@
         <v>20</v>
       </c>
       <c r="C148" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F148" t="s">
         <v>87</v>
@@ -4983,19 +4980,19 @@
         <v>87</v>
       </c>
       <c r="H148" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I148" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J148" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K148" t="s">
         <v>46</v>
       </c>
-      <c r="M148" t="s">
-        <v>9</v>
+      <c r="M148">
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.35">
@@ -5015,19 +5012,19 @@
         <v>87</v>
       </c>
       <c r="H149" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I149" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J149" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K149" t="s">
         <v>46</v>
       </c>
-      <c r="M149">
-        <v>2</v>
+      <c r="M149" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.35">
@@ -5038,7 +5035,7 @@
         <v>20</v>
       </c>
       <c r="C150" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="F150" t="s">
         <v>87</v>
@@ -5047,19 +5044,19 @@
         <v>87</v>
       </c>
       <c r="H150" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I150" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="J150" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K150" t="s">
         <v>46</v>
       </c>
-      <c r="M150" t="s">
-        <v>9</v>
+      <c r="M150">
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.35">
@@ -5099,7 +5096,7 @@
         <v>19</v>
       </c>
       <c r="B152" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="C152" t="s">
         <v>9</v>
@@ -5131,10 +5128,10 @@
         <v>19</v>
       </c>
       <c r="B153" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="C153" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F153" t="s">
         <v>87</v>
@@ -5143,19 +5140,19 @@
         <v>87</v>
       </c>
       <c r="H153" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I153" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="J153" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K153" t="s">
         <v>46</v>
       </c>
-      <c r="M153">
-        <v>1</v>
+      <c r="M153" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.35">
@@ -5163,7 +5160,7 @@
         <v>19</v>
       </c>
       <c r="B154" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C154" t="s">
         <v>37</v>
@@ -5186,16 +5183,25 @@
       <c r="K154" t="s">
         <v>46</v>
       </c>
+      <c r="M154">
+        <v>1</v>
+      </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>8</v>
-      </c>
-      <c r="B155">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="B155" t="s">
+        <v>40</v>
       </c>
       <c r="C155" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="F155" t="s">
+        <v>87</v>
+      </c>
+      <c r="G155" t="s">
+        <v>87</v>
       </c>
       <c r="H155" t="s">
         <v>38</v>
@@ -5209,19 +5215,16 @@
       <c r="K155" t="s">
         <v>46</v>
       </c>
-      <c r="M155">
-        <v>5</v>
-      </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>8</v>
       </c>
       <c r="B156">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C156" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="H156" t="s">
         <v>38</v>
@@ -5236,7 +5239,7 @@
         <v>46</v>
       </c>
       <c r="M156">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.35">
@@ -5247,7 +5250,7 @@
         <v>5</v>
       </c>
       <c r="C157" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H157" t="s">
         <v>38</v>
@@ -5262,39 +5265,33 @@
         <v>46</v>
       </c>
       <c r="M157">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>19</v>
-      </c>
-      <c r="B158" t="s">
-        <v>85</v>
+        <v>8</v>
+      </c>
+      <c r="B158">
+        <v>5</v>
       </c>
       <c r="C158" t="s">
-        <v>9</v>
-      </c>
-      <c r="F158" t="s">
-        <v>87</v>
-      </c>
-      <c r="G158" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="H158" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I158" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="J158" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K158" t="s">
-        <v>80</v>
-      </c>
-      <c r="M158" t="s">
-        <v>9</v>
+        <v>46</v>
+      </c>
+      <c r="M158">
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.35">
@@ -5302,10 +5299,10 @@
         <v>19</v>
       </c>
       <c r="B159" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C159" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F159" t="s">
         <v>87</v>
@@ -5314,19 +5311,19 @@
         <v>87</v>
       </c>
       <c r="H159" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I159" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="J159" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K159" t="s">
-        <v>22</v>
-      </c>
-      <c r="M159">
-        <v>2</v>
+        <v>80</v>
+      </c>
+      <c r="M159" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.35">
@@ -5337,7 +5334,7 @@
         <v>42</v>
       </c>
       <c r="C160" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F160" t="s">
         <v>87</v>
@@ -5358,7 +5355,7 @@
         <v>22</v>
       </c>
       <c r="M160">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.35">
@@ -5369,7 +5366,7 @@
         <v>42</v>
       </c>
       <c r="C161" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F161" t="s">
         <v>87</v>
@@ -5390,7 +5387,7 @@
         <v>22</v>
       </c>
       <c r="M161">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.35">
@@ -5433,7 +5430,7 @@
         <v>42</v>
       </c>
       <c r="C163" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="F163" t="s">
         <v>87</v>
@@ -5442,19 +5439,19 @@
         <v>87</v>
       </c>
       <c r="H163" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I163" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="J163" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="K163" t="s">
-        <v>31</v>
-      </c>
-      <c r="M163" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="M163">
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.35">
@@ -5480,7 +5477,7 @@
         <v>70</v>
       </c>
       <c r="J164" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K164" t="s">
         <v>31</v>
@@ -5526,10 +5523,10 @@
         <v>19</v>
       </c>
       <c r="B166" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C166" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F166" t="s">
         <v>87</v>
@@ -5541,7 +5538,7 @@
         <v>88</v>
       </c>
       <c r="I166" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="J166" t="s">
         <v>73</v>
@@ -5602,19 +5599,19 @@
         <v>87</v>
       </c>
       <c r="H168" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I168" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J168" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K168" t="s">
-        <v>22</v>
-      </c>
-      <c r="M168">
-        <v>7</v>
+        <v>31</v>
+      </c>
+      <c r="M168" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.35">
@@ -5646,7 +5643,7 @@
         <v>22</v>
       </c>
       <c r="M169">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.35">
@@ -5657,7 +5654,7 @@
         <v>20</v>
       </c>
       <c r="C170" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F170" t="s">
         <v>87</v>
@@ -5689,7 +5686,7 @@
         <v>20</v>
       </c>
       <c r="C171" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F171" t="s">
         <v>87</v>
@@ -5710,7 +5707,7 @@
         <v>22</v>
       </c>
       <c r="M171">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.35">
@@ -5721,7 +5718,7 @@
         <v>20</v>
       </c>
       <c r="C172" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F172" t="s">
         <v>87</v>
@@ -5730,19 +5727,19 @@
         <v>87</v>
       </c>
       <c r="H172" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I172" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J172" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K172" t="s">
-        <v>31</v>
-      </c>
-      <c r="M172" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="M172">
+        <v>7</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.35">
@@ -5762,19 +5759,19 @@
         <v>87</v>
       </c>
       <c r="H173" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I173" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J173" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K173" t="s">
-        <v>22</v>
-      </c>
-      <c r="M173">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="M173" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.35">
@@ -5785,7 +5782,7 @@
         <v>20</v>
       </c>
       <c r="C174" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="F174" t="s">
         <v>87</v>
@@ -5797,7 +5794,7 @@
         <v>38</v>
       </c>
       <c r="I174" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J174" t="s">
         <v>7</v>
@@ -5805,11 +5802,8 @@
       <c r="K174" t="s">
         <v>22</v>
       </c>
-      <c r="L174" t="s">
-        <v>23</v>
-      </c>
-      <c r="M174" t="s">
-        <v>9</v>
+      <c r="M174">
+        <v>2</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.35">
@@ -5841,7 +5835,7 @@
         <v>22</v>
       </c>
       <c r="L175" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M175" t="s">
         <v>9</v>
@@ -5876,21 +5870,21 @@
         <v>22</v>
       </c>
       <c r="L176" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M176" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>19</v>
       </c>
       <c r="B177" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="C177" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="F177" t="s">
         <v>87</v>
@@ -5899,22 +5893,25 @@
         <v>87</v>
       </c>
       <c r="H177" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I177" t="s">
         <v>10</v>
       </c>
       <c r="J177" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K177" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="L177" t="s">
+        <v>26</v>
       </c>
       <c r="M177" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>19</v>
       </c>
@@ -5922,7 +5919,7 @@
         <v>85</v>
       </c>
       <c r="C178" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="F178" t="s">
         <v>87</v>
@@ -5934,7 +5931,7 @@
         <v>88</v>
       </c>
       <c r="I178" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="J178" t="s">
         <v>73</v>
@@ -5946,7 +5943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>19</v>
       </c>
@@ -5978,15 +5975,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>19</v>
       </c>
       <c r="B180" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C180" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F180" t="s">
         <v>87</v>
@@ -5998,7 +5995,7 @@
         <v>88</v>
       </c>
       <c r="I180" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="J180" t="s">
         <v>73</v>
@@ -6010,7 +6007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>19</v>
       </c>
@@ -6042,7 +6039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>19</v>
       </c>
@@ -6050,7 +6047,7 @@
         <v>86</v>
       </c>
       <c r="C182" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F182" t="s">
         <v>87</v>
@@ -6074,7 +6071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>19</v>
       </c>
@@ -6106,7 +6103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>19</v>
       </c>
@@ -6138,7 +6135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>19</v>
       </c>
@@ -6146,7 +6143,7 @@
         <v>86</v>
       </c>
       <c r="C185" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F185" t="s">
         <v>87</v>
@@ -6170,7 +6167,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>19</v>
       </c>
@@ -6202,7 +6199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>19</v>
       </c>
@@ -6210,7 +6207,7 @@
         <v>86</v>
       </c>
       <c r="C187" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F187" t="s">
         <v>87</v>
@@ -6234,7 +6231,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>19</v>
       </c>
@@ -6266,7 +6263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>19</v>
       </c>
@@ -6274,7 +6271,7 @@
         <v>86</v>
       </c>
       <c r="C189" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="F189" t="s">
         <v>87</v>
@@ -6286,7 +6283,7 @@
         <v>88</v>
       </c>
       <c r="I189" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="J189" t="s">
         <v>73</v>
@@ -6298,7 +6295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>19</v>
       </c>
@@ -6330,7 +6327,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>19</v>
       </c>
@@ -6353,7 +6350,7 @@
         <v>70</v>
       </c>
       <c r="J191" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K191" t="s">
         <v>31</v>
@@ -6362,15 +6359,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>19</v>
       </c>
       <c r="B192" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="C192" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F192" t="s">
         <v>87</v>
@@ -6379,22 +6376,19 @@
         <v>87</v>
       </c>
       <c r="H192" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I192" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="J192" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="K192" t="s">
-        <v>22</v>
-      </c>
-      <c r="M192">
-        <v>1</v>
-      </c>
-      <c r="N192" t="s">
-        <v>47</v>
+        <v>31</v>
+      </c>
+      <c r="M192" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="193" spans="1:14" x14ac:dyDescent="0.35">
@@ -6426,10 +6420,10 @@
         <v>22</v>
       </c>
       <c r="M193">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N193" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="194" spans="1:14" x14ac:dyDescent="0.35">
@@ -6437,7 +6431,7 @@
         <v>19</v>
       </c>
       <c r="B194" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C194" t="s">
         <v>37</v>
@@ -6461,7 +6455,10 @@
         <v>22</v>
       </c>
       <c r="M194">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="N194" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="195" spans="1:14" x14ac:dyDescent="0.35">
@@ -6472,7 +6469,7 @@
         <v>40</v>
       </c>
       <c r="C195" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F195" t="s">
         <v>87</v>
@@ -6493,10 +6490,7 @@
         <v>22</v>
       </c>
       <c r="M195">
-        <v>2</v>
-      </c>
-      <c r="N195" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="196" spans="1:14" x14ac:dyDescent="0.35">
@@ -6528,7 +6522,10 @@
         <v>22</v>
       </c>
       <c r="M196">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N196" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="197" spans="1:14" x14ac:dyDescent="0.35">
@@ -6539,7 +6536,7 @@
         <v>40</v>
       </c>
       <c r="C197" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F197" t="s">
         <v>87</v>
@@ -6565,13 +6562,19 @@
     </row>
     <row r="198" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>8</v>
-      </c>
-      <c r="B198">
-        <v>4</v>
+        <v>19</v>
+      </c>
+      <c r="B198" t="s">
+        <v>40</v>
       </c>
       <c r="C198" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="F198" t="s">
+        <v>87</v>
+      </c>
+      <c r="G198" t="s">
+        <v>87</v>
       </c>
       <c r="H198" t="s">
         <v>38</v>
@@ -6583,13 +6586,10 @@
         <v>7</v>
       </c>
       <c r="K198" t="s">
-        <v>31</v>
-      </c>
-      <c r="L198" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M198">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:14" x14ac:dyDescent="0.35">
@@ -6600,22 +6600,25 @@
         <v>4</v>
       </c>
       <c r="C199" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="H199" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I199" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J199" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K199" t="s">
         <v>31</v>
       </c>
-      <c r="M199" t="s">
-        <v>9</v>
+      <c r="L199" t="s">
+        <v>23</v>
+      </c>
+      <c r="M199">
+        <v>5</v>
       </c>
     </row>
     <row r="200" spans="1:14" x14ac:dyDescent="0.35">
@@ -6626,7 +6629,7 @@
         <v>4</v>
       </c>
       <c r="C200" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="H200" t="s">
         <v>88</v>
@@ -6649,28 +6652,25 @@
         <v>8</v>
       </c>
       <c r="B201">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C201" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H201" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I201" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J201" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K201" t="s">
-        <v>22</v>
-      </c>
-      <c r="M201">
-        <v>4</v>
-      </c>
-      <c r="N201" t="s">
-        <v>60</v>
+        <v>31</v>
+      </c>
+      <c r="M201" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="202" spans="1:14" x14ac:dyDescent="0.35">
@@ -6696,10 +6696,10 @@
         <v>22</v>
       </c>
       <c r="M202">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N202" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="203" spans="1:14" x14ac:dyDescent="0.35">
@@ -6710,22 +6710,25 @@
         <v>5</v>
       </c>
       <c r="C203" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H203" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I203" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="J203" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="K203" t="s">
-        <v>31</v>
-      </c>
-      <c r="M203" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="M203">
+        <v>1</v>
+      </c>
+      <c r="N203" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="204" spans="1:14" x14ac:dyDescent="0.35">
@@ -6733,7 +6736,7 @@
         <v>8</v>
       </c>
       <c r="B204">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C204" t="s">
         <v>9</v>
@@ -6745,10 +6748,10 @@
         <v>70</v>
       </c>
       <c r="J204" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K204" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="M204" t="s">
         <v>9</v>
@@ -6756,34 +6759,28 @@
     </row>
     <row r="205" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>19</v>
-      </c>
-      <c r="B205" t="s">
-        <v>42</v>
+        <v>8</v>
+      </c>
+      <c r="B205">
+        <v>4</v>
       </c>
       <c r="C205" t="s">
-        <v>37</v>
-      </c>
-      <c r="F205" t="s">
-        <v>87</v>
-      </c>
-      <c r="G205" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="H205" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I205" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="J205" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K205" t="s">
-        <v>39</v>
-      </c>
-      <c r="M205">
-        <v>2</v>
+        <v>81</v>
+      </c>
+      <c r="M205" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="206" spans="1:14" x14ac:dyDescent="0.35">
@@ -6794,7 +6791,7 @@
         <v>42</v>
       </c>
       <c r="C206" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F206" t="s">
         <v>87</v>
@@ -6815,7 +6812,7 @@
         <v>39</v>
       </c>
       <c r="M206">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="207" spans="1:14" x14ac:dyDescent="0.35">
@@ -6823,10 +6820,10 @@
         <v>19</v>
       </c>
       <c r="B207" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C207" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F207" t="s">
         <v>87</v>
@@ -6852,13 +6849,19 @@
     </row>
     <row r="208" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>8</v>
-      </c>
-      <c r="B208">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="B208" t="s">
+        <v>52</v>
       </c>
       <c r="C208" t="s">
-        <v>28</v>
+        <v>37</v>
+      </c>
+      <c r="F208" t="s">
+        <v>87</v>
+      </c>
+      <c r="G208" t="s">
+        <v>87</v>
       </c>
       <c r="H208" t="s">
         <v>38</v>
@@ -6881,10 +6884,10 @@
         <v>8</v>
       </c>
       <c r="B209">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C209" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H209" t="s">
         <v>38</v>
@@ -6904,19 +6907,13 @@
     </row>
     <row r="210" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>19</v>
-      </c>
-      <c r="B210" t="s">
-        <v>42</v>
+        <v>8</v>
+      </c>
+      <c r="B210">
+        <v>5</v>
       </c>
       <c r="C210" t="s">
-        <v>15</v>
-      </c>
-      <c r="F210" t="s">
-        <v>87</v>
-      </c>
-      <c r="G210" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="H210" t="s">
         <v>38</v>
@@ -6928,13 +6925,10 @@
         <v>7</v>
       </c>
       <c r="K210" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="M210">
-        <v>8</v>
-      </c>
-      <c r="N210" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.35">
@@ -6966,10 +6960,10 @@
         <v>25</v>
       </c>
       <c r="M211">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="N211" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="212" spans="1:14" x14ac:dyDescent="0.35">
@@ -6977,7 +6971,7 @@
         <v>19</v>
       </c>
       <c r="B212" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C212" t="s">
         <v>15</v>
@@ -7001,7 +6995,10 @@
         <v>25</v>
       </c>
       <c r="M212">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="N212" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="213" spans="1:14" x14ac:dyDescent="0.35">
@@ -7012,7 +7009,7 @@
         <v>20</v>
       </c>
       <c r="C213" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F213" t="s">
         <v>87</v>
@@ -7033,7 +7030,7 @@
         <v>25</v>
       </c>
       <c r="M213">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="214" spans="1:14" x14ac:dyDescent="0.35">
@@ -7044,7 +7041,7 @@
         <v>20</v>
       </c>
       <c r="C214" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="F214" t="s">
         <v>87</v>
@@ -7056,7 +7053,7 @@
         <v>38</v>
       </c>
       <c r="I214" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J214" t="s">
         <v>7</v>
@@ -7064,8 +7061,8 @@
       <c r="K214" t="s">
         <v>25</v>
       </c>
-      <c r="M214" t="s">
-        <v>9</v>
+      <c r="M214">
+        <v>1</v>
       </c>
     </row>
     <row r="215" spans="1:14" x14ac:dyDescent="0.35">
@@ -7073,10 +7070,10 @@
         <v>19</v>
       </c>
       <c r="B215" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="C215" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F215" t="s">
         <v>87</v>
@@ -7085,16 +7082,16 @@
         <v>87</v>
       </c>
       <c r="H215" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I215" t="s">
         <v>10</v>
       </c>
       <c r="J215" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K215" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M215" t="s">
         <v>9</v>
@@ -7108,7 +7105,7 @@
         <v>86</v>
       </c>
       <c r="C216" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F216" t="s">
         <v>87</v>
@@ -7137,10 +7134,10 @@
         <v>19</v>
       </c>
       <c r="B217" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="C217" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F217" t="s">
         <v>87</v>
@@ -7149,30 +7146,36 @@
         <v>87</v>
       </c>
       <c r="H217" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I217" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J217" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K217" t="s">
-        <v>25</v>
-      </c>
-      <c r="M217">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="M217" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="218" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>8</v>
-      </c>
-      <c r="B218">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="B218" t="s">
+        <v>52</v>
       </c>
       <c r="C218" t="s">
-        <v>15</v>
+        <v>37</v>
+      </c>
+      <c r="F218" t="s">
+        <v>87</v>
+      </c>
+      <c r="G218" t="s">
+        <v>87</v>
       </c>
       <c r="H218" t="s">
         <v>38</v>
@@ -7187,7 +7190,7 @@
         <v>25</v>
       </c>
       <c r="M218">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219" spans="1:14" x14ac:dyDescent="0.35">
@@ -7198,7 +7201,7 @@
         <v>2</v>
       </c>
       <c r="C219" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H219" t="s">
         <v>38</v>
@@ -7213,7 +7216,7 @@
         <v>25</v>
       </c>
       <c r="M219">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="220" spans="1:14" x14ac:dyDescent="0.35">
@@ -7236,10 +7239,10 @@
         <v>7</v>
       </c>
       <c r="K220" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M220">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="221" spans="1:14" x14ac:dyDescent="0.35">
@@ -7247,10 +7250,10 @@
         <v>8</v>
       </c>
       <c r="B221">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C221" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="H221" t="s">
         <v>38</v>
@@ -7262,10 +7265,10 @@
         <v>7</v>
       </c>
       <c r="K221" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="M221">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="222" spans="1:14" x14ac:dyDescent="0.35">
@@ -7273,7 +7276,7 @@
         <v>8</v>
       </c>
       <c r="B222">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C222" t="s">
         <v>15</v>
@@ -7288,10 +7291,10 @@
         <v>7</v>
       </c>
       <c r="K222" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M222">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="223" spans="1:14" x14ac:dyDescent="0.35">
@@ -7299,10 +7302,10 @@
         <v>8</v>
       </c>
       <c r="B223">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C223" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H223" t="s">
         <v>38</v>
@@ -7314,10 +7317,10 @@
         <v>7</v>
       </c>
       <c r="K223" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="M223">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224" spans="1:14" x14ac:dyDescent="0.35">
@@ -7328,7 +7331,7 @@
         <v>5</v>
       </c>
       <c r="C224" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H224" t="s">
         <v>38</v>
@@ -7343,24 +7346,18 @@
         <v>25</v>
       </c>
       <c r="M224">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="225" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>19</v>
-      </c>
-      <c r="B225" t="s">
-        <v>52</v>
+        <v>8</v>
+      </c>
+      <c r="B225">
+        <v>5</v>
       </c>
       <c r="C225" t="s">
-        <v>15</v>
-      </c>
-      <c r="F225" t="s">
-        <v>87</v>
-      </c>
-      <c r="G225" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="H225" t="s">
         <v>38</v>
@@ -7372,13 +7369,10 @@
         <v>7</v>
       </c>
       <c r="K225" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="M225">
-        <v>1</v>
-      </c>
-      <c r="N225" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="226" spans="1:14" x14ac:dyDescent="0.35">
@@ -7389,7 +7383,7 @@
         <v>52</v>
       </c>
       <c r="C226" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F226" t="s">
         <v>87</v>
@@ -7410,19 +7404,28 @@
         <v>53</v>
       </c>
       <c r="M226">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="N226" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="227" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>8</v>
-      </c>
-      <c r="B227">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="B227" t="s">
+        <v>52</v>
       </c>
       <c r="C227" t="s">
         <v>28</v>
       </c>
+      <c r="F227" t="s">
+        <v>87</v>
+      </c>
+      <c r="G227" t="s">
+        <v>87</v>
+      </c>
       <c r="H227" t="s">
         <v>38</v>
       </c>
@@ -7433,10 +7436,10 @@
         <v>7</v>
       </c>
       <c r="K227" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="M227">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="228" spans="1:14" x14ac:dyDescent="0.35">
@@ -7444,10 +7447,10 @@
         <v>8</v>
       </c>
       <c r="B228">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C228" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H228" t="s">
         <v>38</v>
@@ -7462,10 +7465,7 @@
         <v>61</v>
       </c>
       <c r="M228">
-        <v>2</v>
-      </c>
-      <c r="N228" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229" spans="1:14" x14ac:dyDescent="0.35">
@@ -7473,10 +7473,10 @@
         <v>8</v>
       </c>
       <c r="B229">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C229" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H229" t="s">
         <v>38</v>
@@ -7488,42 +7488,39 @@
         <v>7</v>
       </c>
       <c r="K229" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="M229">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N229" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="230" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>19</v>
-      </c>
-      <c r="B230" t="s">
-        <v>42</v>
+        <v>8</v>
+      </c>
+      <c r="B230">
+        <v>3</v>
       </c>
       <c r="C230" t="s">
-        <v>9</v>
-      </c>
-      <c r="F230" t="s">
-        <v>87</v>
-      </c>
-      <c r="G230" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="H230" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I230" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="J230" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="K230" t="s">
-        <v>82</v>
-      </c>
-      <c r="M230" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="M230">
+        <v>1</v>
       </c>
     </row>
     <row r="231" spans="1:14" x14ac:dyDescent="0.35">
@@ -7534,7 +7531,7 @@
         <v>42</v>
       </c>
       <c r="C231" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F231" t="s">
         <v>87</v>
@@ -7543,19 +7540,19 @@
         <v>87</v>
       </c>
       <c r="H231" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="I231" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="J231" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="K231" t="s">
-        <v>67</v>
-      </c>
-      <c r="M231">
-        <v>1</v>
+        <v>82</v>
+      </c>
+      <c r="M231" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="232" spans="1:14" x14ac:dyDescent="0.35">
@@ -7563,10 +7560,10 @@
         <v>19</v>
       </c>
       <c r="B232" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="C232" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F232" t="s">
         <v>87</v>
@@ -7575,19 +7572,19 @@
         <v>87</v>
       </c>
       <c r="H232" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="I232" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="J232" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K232" t="s">
-        <v>83</v>
-      </c>
-      <c r="M232" t="s">
-        <v>9</v>
+        <v>67</v>
+      </c>
+      <c r="M232">
+        <v>1</v>
       </c>
     </row>
     <row r="233" spans="1:14" x14ac:dyDescent="0.35">
@@ -7595,36 +7592,68 @@
         <v>19</v>
       </c>
       <c r="B233" t="s">
+        <v>85</v>
+      </c>
+      <c r="C233" t="s">
+        <v>9</v>
+      </c>
+      <c r="F233" t="s">
+        <v>87</v>
+      </c>
+      <c r="G233" t="s">
+        <v>87</v>
+      </c>
+      <c r="H233" t="s">
+        <v>88</v>
+      </c>
+      <c r="I233" t="s">
+        <v>70</v>
+      </c>
+      <c r="J233" t="s">
+        <v>73</v>
+      </c>
+      <c r="K233" t="s">
+        <v>83</v>
+      </c>
+      <c r="M233" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="234" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
+        <v>19</v>
+      </c>
+      <c r="B234" t="s">
         <v>52</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C234" t="s">
         <v>28</v>
       </c>
-      <c r="F233" t="s">
-        <v>87</v>
-      </c>
-      <c r="G233" t="s">
-        <v>87</v>
-      </c>
-      <c r="H233" t="s">
-        <v>38</v>
-      </c>
-      <c r="I233" t="s">
-        <v>16</v>
-      </c>
-      <c r="J233" t="s">
-        <v>7</v>
-      </c>
-      <c r="K233" t="s">
+      <c r="F234" t="s">
+        <v>87</v>
+      </c>
+      <c r="G234" t="s">
+        <v>87</v>
+      </c>
+      <c r="H234" t="s">
+        <v>38</v>
+      </c>
+      <c r="I234" t="s">
+        <v>16</v>
+      </c>
+      <c r="J234" t="s">
+        <v>7</v>
+      </c>
+      <c r="K234" t="s">
         <v>90</v>
       </c>
-      <c r="M233">
+      <c r="M234">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N233">
-    <sortCondition ref="K2:K233"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N234">
+    <sortCondition ref="K2:K234"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>